<commit_message>
Updated monitored URLs list
</commit_message>
<xml_diff>
--- a/data/urls.xlsx
+++ b/data/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A866AF-D555-4604-BE20-DC12198AB061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAFA096-AE6C-4A22-AA41-014EDCD14171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>https://your-site.com</t>
   </si>
   <si>
-    <t>https://atpsgroup.com/dahshs</t>
+    <t>https://myactivity.in/adhasha</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="A1:XFD1048576"/>
+      <selection activeCell="A9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +423,6 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{A6C9724D-2BB6-4042-9B27-2A4E08F6625C}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{5B0089DD-9184-4205-8EFC-9236BF8F62BB}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{59808F38-EC80-4A13-8635-64D8016DF5B6}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{45A8EA50-48B9-48E1-969E-45D07B982B1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new excel added for testing webhook
</commit_message>
<xml_diff>
--- a/data/urls.xlsx
+++ b/data/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAFA096-AE6C-4A22-AA41-014EDCD14171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BE5F8F-51D6-40F2-B230-4CFCD8E3EDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>https://your-site.com</t>
   </si>
   <si>
-    <t>https://myactivity.in/adhasha</t>
+    <t>https://atpsgroup.com/admin/helloworld</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+      <selection activeCell="A5" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
testing the extended email stuff from jenkins
</commit_message>
<xml_diff>
--- a/data/urls.xlsx
+++ b/data/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BE5F8F-51D6-40F2-B230-4CFCD8E3EDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB400C-2B34-4D13-9E1F-D6BD3AF6EF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>https://your-site.com</t>
   </si>
   <si>
-    <t>https://atpsgroup.com/admin/helloworld</t>
+    <t>https://atpsgroup.com/admin/helloworld001</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:A5"/>
+      <selection activeCell="G10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,6 +423,7 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{A6C9724D-2BB6-4042-9B27-2A4E08F6625C}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{5B0089DD-9184-4205-8EFC-9236BF8F62BB}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{59808F38-EC80-4A13-8635-64D8016DF5B6}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{B339D875-8212-4743-93ED-C5FDFC392CDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new set of urls with 1 failed url
</commit_message>
<xml_diff>
--- a/data/urls.xlsx
+++ b/data/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB400C-2B34-4D13-9E1F-D6BD3AF6EF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F785954-B698-456F-9A2E-31FC1AF00341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>https://your-site.com</t>
   </si>
   <si>
-    <t>https://atpsgroup.com/admin/helloworld001</t>
+    <t>https://atpsgroup.com/admin/helloworldtest</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="A1:XFD1048576"/>
+      <selection activeCell="C13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
new set of urls
</commit_message>
<xml_diff>
--- a/data/urls.xlsx
+++ b/data/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F785954-B698-456F-9A2E-31FC1AF00341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6719D0E3-FDF4-46A3-8468-E63DC4F85FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>https://your-site.com</t>
   </si>
   <si>
-    <t>https://atpsgroup.com/admin/helloworldtest</t>
+    <t>https://atpsgroup.com/admin/helloworldtesting</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="A1:XFD1048576"/>
+      <selection activeCell="A17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
new url with errorisalliwant
</commit_message>
<xml_diff>
--- a/data/urls.xlsx
+++ b/data/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6719D0E3-FDF4-46A3-8468-E63DC4F85FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0762B6F-A874-4BC3-A4C5-DE0C4BCD0A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>https://your-site.com</t>
   </si>
   <si>
-    <t>https://atpsgroup.com/admin/helloworldtesting</t>
+    <t>http://www.atpsgroup.com/erroriswhatweneeed</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A1:XFD1048576"/>
+      <selection activeCell="A12" activeCellId="1" sqref="A5 A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +423,7 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{A6C9724D-2BB6-4042-9B27-2A4E08F6625C}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{5B0089DD-9184-4205-8EFC-9236BF8F62BB}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{59808F38-EC80-4A13-8635-64D8016DF5B6}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{B339D875-8212-4743-93ED-C5FDFC392CDF}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{A4E20934-BE34-403F-8CB0-8C6D14AFE754}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>